<commit_message>
Added Free FB and updated gen to 4 for youtube
</commit_message>
<xml_diff>
--- a/Application.xlsx
+++ b/Application.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ncellaxiata-my.sharepoint.com/personal/amul_joshi_ncell_com_np/Documents/Documents/SCRIPT_GENERATOR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ncellnp-my.sharepoint.com/personal/amul_joshi_ncell_com_np/Documents/Documents/SCRIPT_GENERATOR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="11_F25DC773A252ABDACC104877F95952F05BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA3F5499-4046-497E-A203-98A762F11929}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="11_F25DC773A252ABDACC104877F95952F05BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{907182DB-BDB6-4B81-AB9C-7B2D0BEA8FDF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -112,6 +123,36 @@
   </si>
   <si>
     <t>fg_zoom</t>
+  </si>
+  <si>
+    <t>FreeFacebook</t>
+  </si>
+  <si>
+    <t>f_freefbip_</t>
+  </si>
+  <si>
+    <t>fg_freefbip</t>
+  </si>
+  <si>
+    <t>FreeFacebook-IPV6</t>
+  </si>
+  <si>
+    <t>f_freefbipv6_</t>
+  </si>
+  <si>
+    <t>Facebook Header</t>
+  </si>
+  <si>
+    <t>f_fbheaderip_</t>
+  </si>
+  <si>
+    <t>fg_fbheaderip</t>
+  </si>
+  <si>
+    <t>Facebook Header-IPV6</t>
+  </si>
+  <si>
+    <t>f_fbheaderipv6_</t>
   </si>
 </sst>
 </file>
@@ -147,9 +188,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,22 +470,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -470,115 +510,115 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -595,7 +635,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -612,7 +652,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -629,8 +669,73 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H12" s="1"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>